<commit_message>
initial test seems to work to populate cell by range
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Basic_Excel_2cells.xlsx
+++ b/test/fixtures/files/Basic_Excel_2cells.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="5500" windowWidth="25600" windowHeight="18100" tabRatio="500"/>
+    <workbookView xWindow="4860" yWindow="2780" windowWidth="25600" windowHeight="18100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Cell_1">Sheet1!$B$3</definedName>
+    <definedName name="cell1rangename">Sheet1!$C$3</definedName>
+    <definedName name="cell2rangename">Sheet1!$F$6</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,38 +23,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Cell_1</t>
+    <t>Cell1</t>
   </si>
   <si>
-    <t>Cell_2</t>
+    <t>oldvalue</t>
+  </si>
+  <si>
+    <t>Cell2</t>
+  </si>
+  <si>
+    <t>oldvalue2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,17 +67,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,30 +403,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D5"/>
+  <dimension ref="B3:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="C5" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>1</v>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>